<commit_message>
Update for fHarvest* var. Note that in checkvars the --nemo label seems to has lost its meaning, probably since the realm check has been dropped, this has the consequence that the nemo-miss file includes all missing instead of nemo-only missing.
</commit_message>
<xml_diff>
--- a/ece2cmor3/scripts/create-nemo-only-list/nemo-miss-list-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/scripts/create-nemo-only-list/nemo-miss-list-cmpi6-requested-variables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7023" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7032" uniqueCount="1888">
   <si>
     <t>Table</t>
   </si>
@@ -4763,6 +4763,15 @@
   </si>
   <si>
     <t>Dissolved inorganic carbon-14 (CO3+HCO3+H2CO3) concentration</t>
+  </si>
+  <si>
+    <t>fHarvestToProduct</t>
+  </si>
+  <si>
+    <t>Harvested Biomass That Goes into Product Pool</t>
+  </si>
+  <si>
+    <t>be it food or wood harvest, any carbon that is subsequently stored is reported here</t>
   </si>
   <si>
     <t>fN2O</t>
@@ -6009,7 +6018,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N813"/>
+  <dimension ref="A1:N814"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -26681,14 +26690,14 @@
         <v>202</v>
       </c>
       <c r="G657">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912cf78-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J657" t="s">
         <v>1585</v>
       </c>
       <c r="K657" t="s">
-        <v>1475</v>
+        <v>1500</v>
       </c>
       <c r="M657" t="s">
         <v>202</v>
@@ -26702,7 +26711,7 @@
         <v>1586</v>
       </c>
       <c r="C658" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D658" t="s">
         <v>172</v>
@@ -26714,14 +26723,14 @@
         <v>202</v>
       </c>
       <c r="G658">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f097e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912cf78-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J658" t="s">
         <v>1588</v>
       </c>
       <c r="K658" t="s">
-        <v>1500</v>
+        <v>1475</v>
       </c>
       <c r="M658" t="s">
         <v>202</v>
@@ -26735,7 +26744,7 @@
         <v>1589</v>
       </c>
       <c r="C659" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D659" t="s">
         <v>172</v>
@@ -26747,7 +26756,7 @@
         <v>202</v>
       </c>
       <c r="G659">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912d5ea-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f097e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J659" t="s">
@@ -26768,7 +26777,7 @@
         <v>1592</v>
       </c>
       <c r="C660" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D660" t="s">
         <v>172</v>
@@ -26780,7 +26789,7 @@
         <v>202</v>
       </c>
       <c r="G660">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913a696-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912d5ea-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J660" t="s">
@@ -26813,11 +26822,11 @@
         <v>202</v>
       </c>
       <c r="G661">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591348fe-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913a696-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J661" t="s">
-        <v>1594</v>
+        <v>1597</v>
       </c>
       <c r="K661" t="s">
         <v>1500</v>
@@ -26831,7 +26840,7 @@
         <v>1467</v>
       </c>
       <c r="B662" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="C662" t="s">
         <v>55</v>
@@ -26840,17 +26849,17 @@
         <v>172</v>
       </c>
       <c r="E662" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="F662" t="s">
         <v>202</v>
       </c>
       <c r="G662">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84ef402c-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591348fe-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J662" t="s">
-        <v>1594</v>
+        <v>1597</v>
       </c>
       <c r="K662" t="s">
         <v>1500</v>
@@ -26864,7 +26873,7 @@
         <v>1467</v>
       </c>
       <c r="B663" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
       <c r="C663" t="s">
         <v>55</v>
@@ -26873,17 +26882,17 @@
         <v>172</v>
       </c>
       <c r="E663" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="F663" t="s">
         <v>202</v>
       </c>
       <c r="G663">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0ddec-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84ef402c-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J663" t="s">
-        <v>1594</v>
+        <v>1597</v>
       </c>
       <c r="K663" t="s">
         <v>1500</v>
@@ -26897,32 +26906,32 @@
         <v>1467</v>
       </c>
       <c r="B664" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="C664" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D664" t="s">
-        <v>1602</v>
+        <v>172</v>
       </c>
       <c r="E664" t="s">
         <v>1603</v>
       </c>
       <c r="F664" t="s">
-        <v>95</v>
+        <v>202</v>
       </c>
       <c r="G664">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3f30557c-b89b-11e6-be04-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0ddec-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J664" t="s">
-        <v>1604</v>
+        <v>1597</v>
       </c>
       <c r="K664" t="s">
-        <v>1605</v>
+        <v>1500</v>
       </c>
       <c r="M664" t="s">
-        <v>95</v>
+        <v>202</v>
       </c>
     </row>
     <row r="665" spans="1:13">
@@ -26930,32 +26939,32 @@
         <v>1467</v>
       </c>
       <c r="B665" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C665" t="s">
+        <v>35</v>
+      </c>
+      <c r="D665" t="s">
+        <v>1605</v>
+      </c>
+      <c r="E665" t="s">
         <v>1606</v>
       </c>
-      <c r="C665" t="s">
-        <v>55</v>
-      </c>
-      <c r="D665" t="s">
-        <v>172</v>
-      </c>
-      <c r="E665" t="s">
+      <c r="F665" t="s">
+        <v>95</v>
+      </c>
+      <c r="G665">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3f30557c-b89b-11e6-be04-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J665" t="s">
         <v>1607</v>
       </c>
-      <c r="F665" t="s">
-        <v>202</v>
-      </c>
-      <c r="G665">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917788e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J665" t="s">
+      <c r="K665" t="s">
         <v>1608</v>
       </c>
-      <c r="K665" t="s">
-        <v>1475</v>
-      </c>
       <c r="M665" t="s">
-        <v>202</v>
+        <v>95</v>
       </c>
     </row>
     <row r="666" spans="1:13">
@@ -26978,14 +26987,14 @@
         <v>202</v>
       </c>
       <c r="G666">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0c47e-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917788e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J666" t="s">
         <v>1611</v>
       </c>
       <c r="K666" t="s">
-        <v>1500</v>
+        <v>1475</v>
       </c>
       <c r="M666" t="s">
         <v>202</v>
@@ -27011,14 +27020,14 @@
         <v>202</v>
       </c>
       <c r="G667">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f9ace-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0c47e-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J667" t="s">
         <v>1614</v>
       </c>
       <c r="K667" t="s">
-        <v>1475</v>
+        <v>1500</v>
       </c>
       <c r="M667" t="s">
         <v>202</v>
@@ -27044,7 +27053,7 @@
         <v>202</v>
       </c>
       <c r="G668">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f95c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f9ace-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J668" t="s">
@@ -27062,32 +27071,32 @@
         <v>1467</v>
       </c>
       <c r="B669" t="s">
-        <v>1319</v>
+        <v>1618</v>
       </c>
       <c r="C669" t="s">
         <v>55</v>
       </c>
       <c r="D669" t="s">
-        <v>1542</v>
+        <v>172</v>
       </c>
       <c r="E669" t="s">
-        <v>1320</v>
+        <v>1619</v>
       </c>
       <c r="F669" t="s">
-        <v>35</v>
+        <v>202</v>
       </c>
       <c r="G669">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f21d4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f95c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J669" t="s">
-        <v>1321</v>
+        <v>1620</v>
       </c>
       <c r="K669" t="s">
-        <v>21</v>
+        <v>1475</v>
       </c>
       <c r="M669" t="s">
-        <v>35</v>
+        <v>202</v>
       </c>
     </row>
     <row r="670" spans="1:13">
@@ -27095,32 +27104,32 @@
         <v>1467</v>
       </c>
       <c r="B670" t="s">
-        <v>1618</v>
+        <v>1319</v>
       </c>
       <c r="C670" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D670" t="s">
-        <v>1602</v>
+        <v>1542</v>
       </c>
       <c r="E670" t="s">
-        <v>1619</v>
+        <v>1320</v>
       </c>
       <c r="F670" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="G670">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ee804-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f21d4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J670" t="s">
-        <v>1620</v>
+        <v>1321</v>
       </c>
       <c r="K670" t="s">
-        <v>1605</v>
+        <v>21</v>
       </c>
       <c r="M670" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
     </row>
     <row r="671" spans="1:13">
@@ -27134,7 +27143,7 @@
         <v>35</v>
       </c>
       <c r="D671" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
       <c r="E671" t="s">
         <v>1622</v>
@@ -27143,14 +27152,14 @@
         <v>95</v>
       </c>
       <c r="G671">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e590c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ee804-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J671" t="s">
         <v>1623</v>
       </c>
       <c r="K671" t="s">
-        <v>1605</v>
+        <v>1608</v>
       </c>
       <c r="M671" t="s">
         <v>95</v>
@@ -27161,32 +27170,32 @@
         <v>1467</v>
       </c>
       <c r="B672" t="s">
-        <v>1348</v>
+        <v>1624</v>
       </c>
       <c r="C672" t="s">
         <v>35</v>
       </c>
       <c r="D672" t="s">
-        <v>1349</v>
+        <v>1605</v>
       </c>
       <c r="E672" t="s">
-        <v>1350</v>
+        <v>1625</v>
       </c>
       <c r="F672" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="G672">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bf56baca-c14c-11e6-bb6a-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e590c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J672" t="s">
-        <v>1351</v>
+        <v>1626</v>
       </c>
       <c r="K672" t="s">
-        <v>1048</v>
+        <v>1608</v>
       </c>
       <c r="M672" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="673" spans="1:13">
@@ -27194,32 +27203,32 @@
         <v>1467</v>
       </c>
       <c r="B673" t="s">
-        <v>1624</v>
+        <v>1348</v>
       </c>
       <c r="C673" t="s">
         <v>35</v>
       </c>
       <c r="D673" t="s">
-        <v>1625</v>
+        <v>1349</v>
       </c>
       <c r="E673" t="s">
-        <v>1626</v>
+        <v>1350</v>
       </c>
       <c r="F673" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G673">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59178a72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bf56baca-c14c-11e6-bb6a-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J673" t="s">
-        <v>1627</v>
+        <v>1351</v>
       </c>
       <c r="K673" t="s">
-        <v>1605</v>
+        <v>1048</v>
       </c>
       <c r="M673" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="674" spans="1:13">
@@ -27227,32 +27236,32 @@
         <v>1467</v>
       </c>
       <c r="B674" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C674" t="s">
+        <v>35</v>
+      </c>
+      <c r="D674" t="s">
         <v>1628</v>
-      </c>
-      <c r="C674" t="s">
-        <v>35</v>
-      </c>
-      <c r="D674" t="s">
-        <v>172</v>
       </c>
       <c r="E674" t="s">
         <v>1629</v>
       </c>
       <c r="F674" t="s">
+        <v>35</v>
+      </c>
+      <c r="G674">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59178a72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J674" t="s">
         <v>1630</v>
       </c>
-      <c r="G674">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J674" t="s">
-        <v>1631</v>
-      </c>
       <c r="K674" t="s">
-        <v>1471</v>
+        <v>1608</v>
       </c>
       <c r="M674" t="s">
-        <v>1630</v>
+        <v>35</v>
       </c>
     </row>
     <row r="675" spans="1:13">
@@ -27260,7 +27269,7 @@
         <v>1467</v>
       </c>
       <c r="B675" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="C675" t="s">
         <v>35</v>
@@ -27269,23 +27278,23 @@
         <v>172</v>
       </c>
       <c r="E675" t="s">
+        <v>1632</v>
+      </c>
+      <c r="F675" t="s">
         <v>1633</v>
       </c>
-      <c r="F675" t="s">
+      <c r="G675">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917acf0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J675" t="s">
         <v>1634</v>
-      </c>
-      <c r="G675">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J675" t="s">
-        <v>1635</v>
       </c>
       <c r="K675" t="s">
         <v>1471</v>
       </c>
       <c r="M675" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="676" spans="1:13">
@@ -27293,7 +27302,7 @@
         <v>1467</v>
       </c>
       <c r="B676" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C676" t="s">
         <v>35</v>
@@ -27302,13 +27311,13 @@
         <v>172</v>
       </c>
       <c r="E676" t="s">
+        <v>1636</v>
+      </c>
+      <c r="F676" t="s">
         <v>1637</v>
       </c>
-      <c r="F676" t="s">
-        <v>1630</v>
-      </c>
       <c r="G676">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590de58a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J676" t="s">
@@ -27318,7 +27327,7 @@
         <v>1471</v>
       </c>
       <c r="M676" t="s">
-        <v>1630</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="677" spans="1:13">
@@ -27338,10 +27347,10 @@
         <v>1640</v>
       </c>
       <c r="F677" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="G677">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147b48-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J677" t="s">
@@ -27351,7 +27360,7 @@
         <v>1471</v>
       </c>
       <c r="M677" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="678" spans="1:13">
@@ -27359,32 +27368,32 @@
         <v>1467</v>
       </c>
       <c r="B678" t="s">
-        <v>1171</v>
+        <v>1642</v>
       </c>
       <c r="C678" t="s">
         <v>35</v>
       </c>
       <c r="D678" t="s">
-        <v>1352</v>
+        <v>172</v>
       </c>
       <c r="E678" t="s">
-        <v>1173</v>
+        <v>1643</v>
       </c>
       <c r="F678" t="s">
-        <v>42</v>
+        <v>1637</v>
       </c>
       <c r="G678">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59149a10-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591444ca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J678" t="s">
-        <v>1174</v>
+        <v>1644</v>
       </c>
       <c r="K678" t="s">
-        <v>1152</v>
+        <v>1471</v>
       </c>
       <c r="M678" t="s">
-        <v>42</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="679" spans="1:13">
@@ -27392,26 +27401,26 @@
         <v>1467</v>
       </c>
       <c r="B679" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="C679" t="s">
         <v>35</v>
       </c>
       <c r="D679" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="E679" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="F679" t="s">
         <v>42</v>
       </c>
       <c r="G679">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912eff8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59149a10-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J679" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="K679" t="s">
         <v>1152</v>
@@ -27425,32 +27434,32 @@
         <v>1467</v>
       </c>
       <c r="B680" t="s">
-        <v>1369</v>
+        <v>1175</v>
       </c>
       <c r="C680" t="s">
         <v>35</v>
       </c>
       <c r="D680" t="s">
-        <v>172</v>
+        <v>1353</v>
       </c>
       <c r="E680" t="s">
-        <v>1370</v>
+        <v>1177</v>
       </c>
       <c r="F680" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G680">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912eff8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J680" t="s">
-        <v>1371</v>
+        <v>1178</v>
       </c>
       <c r="K680" t="s">
-        <v>1547</v>
+        <v>1152</v>
       </c>
       <c r="M680" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="681" spans="1:13">
@@ -27458,7 +27467,7 @@
         <v>1467</v>
       </c>
       <c r="B681" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="C681" t="s">
         <v>35</v>
@@ -27467,17 +27476,17 @@
         <v>172</v>
       </c>
       <c r="E681" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="F681" t="s">
         <v>50</v>
       </c>
       <c r="G681">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a17b2a3bcad6c41455a7e2474fb1fdcb.html","web")</f>
         <v>0</v>
       </c>
       <c r="J681" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="K681" t="s">
         <v>1547</v>
@@ -27491,7 +27500,7 @@
         <v>1467</v>
       </c>
       <c r="B682" t="s">
-        <v>1642</v>
+        <v>1375</v>
       </c>
       <c r="C682" t="s">
         <v>35</v>
@@ -27500,23 +27509,23 @@
         <v>172</v>
       </c>
       <c r="E682" t="s">
-        <v>1643</v>
+        <v>1376</v>
       </c>
       <c r="F682" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G682">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914ede4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d9deb887c24ae8008ca2179208f99d.html","web")</f>
         <v>0</v>
       </c>
       <c r="J682" t="s">
-        <v>1644</v>
+        <v>1377</v>
       </c>
       <c r="K682" t="s">
-        <v>1471</v>
+        <v>1547</v>
       </c>
       <c r="M682" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="683" spans="1:13">
@@ -27539,7 +27548,7 @@
         <v>95</v>
       </c>
       <c r="G683">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591497a4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914ede4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J683" t="s">
@@ -27572,7 +27581,7 @@
         <v>95</v>
       </c>
       <c r="G684">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f9f66ff437154f86913937f9e2d9a26d.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591497a4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J684" t="s">
@@ -27605,11 +27614,11 @@
         <v>95</v>
       </c>
       <c r="G685">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ab57604d6acd918c08aa6252145c608e.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f9f66ff437154f86913937f9e2d9a26d.html","web")</f>
         <v>0</v>
       </c>
       <c r="J685" t="s">
-        <v>1650</v>
+        <v>1653</v>
       </c>
       <c r="K685" t="s">
         <v>1471</v>
@@ -27623,7 +27632,7 @@
         <v>1467</v>
       </c>
       <c r="B686" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="C686" t="s">
         <v>35</v>
@@ -27632,17 +27641,17 @@
         <v>172</v>
       </c>
       <c r="E686" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="F686" t="s">
         <v>95</v>
       </c>
       <c r="G686">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59134bf6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ab57604d6acd918c08aa6252145c608e.html","web")</f>
         <v>0</v>
       </c>
       <c r="J686" t="s">
-        <v>1644</v>
+        <v>1653</v>
       </c>
       <c r="K686" t="s">
         <v>1471</v>
@@ -27656,7 +27665,7 @@
         <v>1467</v>
       </c>
       <c r="B687" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="C687" t="s">
         <v>35</v>
@@ -27665,23 +27674,23 @@
         <v>172</v>
       </c>
       <c r="E687" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="F687" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="G687">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59130e98-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59134bf6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J687" t="s">
-        <v>1657</v>
+        <v>1647</v>
       </c>
       <c r="K687" t="s">
-        <v>1475</v>
+        <v>1471</v>
       </c>
       <c r="M687" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="688" spans="1:13">
@@ -27689,26 +27698,26 @@
         <v>1467</v>
       </c>
       <c r="B688" t="s">
-        <v>1378</v>
+        <v>1658</v>
       </c>
       <c r="C688" t="s">
         <v>35</v>
       </c>
       <c r="D688" t="s">
-        <v>1379</v>
+        <v>172</v>
       </c>
       <c r="E688" t="s">
-        <v>1380</v>
+        <v>1659</v>
       </c>
       <c r="F688" t="s">
         <v>50</v>
       </c>
       <c r="G688">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590d17f4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59130e98-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J688" t="s">
-        <v>1381</v>
+        <v>1660</v>
       </c>
       <c r="K688" t="s">
         <v>1475</v>
@@ -27722,26 +27731,26 @@
         <v>1467</v>
       </c>
       <c r="B689" t="s">
-        <v>1658</v>
+        <v>1378</v>
       </c>
       <c r="C689" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D689" t="s">
-        <v>172</v>
+        <v>1379</v>
       </c>
       <c r="E689" t="s">
-        <v>1659</v>
+        <v>1380</v>
       </c>
       <c r="F689" t="s">
         <v>50</v>
       </c>
       <c r="G689">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590d24c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590d17f4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J689" t="s">
-        <v>1660</v>
+        <v>1381</v>
       </c>
       <c r="K689" t="s">
         <v>1475</v>
@@ -27767,10 +27776,10 @@
         <v>1662</v>
       </c>
       <c r="F690" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
       <c r="G690">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59176d94-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590d24c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J690" t="s">
@@ -27780,7 +27789,7 @@
         <v>1475</v>
       </c>
       <c r="M690" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
     </row>
     <row r="691" spans="1:13">
@@ -27803,7 +27812,7 @@
         <v>202</v>
       </c>
       <c r="G691">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59132b58-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59176d94-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J691" t="s">
@@ -27836,14 +27845,14 @@
         <v>202</v>
       </c>
       <c r="G692">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0bbbe-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59132b58-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J692" t="s">
         <v>1669</v>
       </c>
       <c r="K692" t="s">
-        <v>1500</v>
+        <v>1475</v>
       </c>
       <c r="M692" t="s">
         <v>202</v>
@@ -27869,7 +27878,7 @@
         <v>202</v>
       </c>
       <c r="G693">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0f052-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0bbbe-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J693" t="s">
@@ -27902,11 +27911,11 @@
         <v>202</v>
       </c>
       <c r="G694">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f09f30-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0f052-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J694" t="s">
-        <v>1669</v>
+        <v>1675</v>
       </c>
       <c r="K694" t="s">
         <v>1500</v>
@@ -27920,32 +27929,32 @@
         <v>1467</v>
       </c>
       <c r="B695" t="s">
-        <v>216</v>
+        <v>1676</v>
       </c>
       <c r="C695" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D695" t="s">
         <v>172</v>
       </c>
       <c r="E695" t="s">
-        <v>217</v>
+        <v>1677</v>
       </c>
       <c r="F695" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="G695">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/117c89cc-b574-11e6-9ed4-5404a60d96b5.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f09f30-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J695" t="s">
-        <v>219</v>
+        <v>1672</v>
       </c>
       <c r="K695" t="s">
-        <v>1675</v>
+        <v>1500</v>
       </c>
       <c r="M695" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
     </row>
     <row r="696" spans="1:13">
@@ -27953,32 +27962,32 @@
         <v>1467</v>
       </c>
       <c r="B696" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C696" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D696" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="E696" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F696" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
       <c r="G696">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1742f769c80d35356bf80ab91789eec6.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/117c89cc-b574-11e6-9ed4-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="J696" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K696" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M696" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
     </row>
     <row r="697" spans="1:13">
@@ -27986,32 +27995,32 @@
         <v>1467</v>
       </c>
       <c r="B697" t="s">
-        <v>1676</v>
+        <v>220</v>
       </c>
       <c r="C697" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D697" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="E697" t="s">
-        <v>1677</v>
+        <v>221</v>
       </c>
       <c r="F697" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="G697">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59130948-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1742f769c80d35356bf80ab91789eec6.html","web")</f>
         <v>0</v>
       </c>
       <c r="J697" t="s">
+        <v>222</v>
+      </c>
+      <c r="K697" t="s">
         <v>1678</v>
       </c>
-      <c r="K697" t="s">
-        <v>1471</v>
-      </c>
       <c r="M697" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
     </row>
     <row r="698" spans="1:13">
@@ -28025,7 +28034,7 @@
         <v>35</v>
       </c>
       <c r="D698" t="s">
-        <v>1094</v>
+        <v>172</v>
       </c>
       <c r="E698" t="s">
         <v>1680</v>
@@ -28034,14 +28043,14 @@
         <v>35</v>
       </c>
       <c r="G698">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59130948-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J698" t="s">
         <v>1681</v>
       </c>
       <c r="K698" t="s">
-        <v>1682</v>
+        <v>1471</v>
       </c>
       <c r="M698" t="s">
         <v>35</v>
@@ -28052,7 +28061,7 @@
         <v>1467</v>
       </c>
       <c r="B699" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="C699" t="s">
         <v>35</v>
@@ -28061,20 +28070,20 @@
         <v>1094</v>
       </c>
       <c r="E699" t="s">
+        <v>1683</v>
+      </c>
+      <c r="F699" t="s">
+        <v>35</v>
+      </c>
+      <c r="G699">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591720a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J699" t="s">
         <v>1684</v>
       </c>
-      <c r="F699" t="s">
-        <v>35</v>
-      </c>
-      <c r="G699">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914cf30-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J699" t="s">
+      <c r="K699" t="s">
         <v>1685</v>
-      </c>
-      <c r="K699" t="s">
-        <v>1471</v>
       </c>
       <c r="M699" t="s">
         <v>35</v>
@@ -28091,7 +28100,7 @@
         <v>35</v>
       </c>
       <c r="D700" t="s">
-        <v>172</v>
+        <v>1094</v>
       </c>
       <c r="E700" t="s">
         <v>1687</v>
@@ -28100,7 +28109,7 @@
         <v>35</v>
       </c>
       <c r="G700">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914c0ee-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914cf30-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J700" t="s">
@@ -28118,32 +28127,32 @@
         <v>1467</v>
       </c>
       <c r="B701" t="s">
-        <v>223</v>
+        <v>1689</v>
       </c>
       <c r="C701" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D701" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="E701" t="s">
-        <v>224</v>
+        <v>1690</v>
       </c>
       <c r="F701" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="G701">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2aa31f177542022b5d6ca809cf01eff5.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914c0ee-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J701" t="s">
-        <v>225</v>
+        <v>1691</v>
       </c>
       <c r="K701" t="s">
-        <v>1675</v>
+        <v>1471</v>
       </c>
       <c r="M701" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
     </row>
     <row r="702" spans="1:13">
@@ -28151,32 +28160,32 @@
         <v>1467</v>
       </c>
       <c r="B702" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C702" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D702" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="E702" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F702" t="s">
-        <v>218</v>
+        <v>95</v>
       </c>
       <c r="G702">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59133ddc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2aa31f177542022b5d6ca809cf01eff5.html","web")</f>
         <v>0</v>
       </c>
       <c r="J702" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K702" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M702" t="s">
-        <v>218</v>
+        <v>95</v>
       </c>
     </row>
     <row r="703" spans="1:13">
@@ -28184,32 +28193,32 @@
         <v>1467</v>
       </c>
       <c r="B703" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C703" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D703" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="E703" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F703" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
       <c r="G703">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8530ec1d1281da71f660df7c61571e38.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59133ddc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J703" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K703" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M703" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
     </row>
     <row r="704" spans="1:13">
@@ -28217,7 +28226,7 @@
         <v>1467</v>
       </c>
       <c r="B704" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C704" t="s">
         <v>55</v>
@@ -28226,20 +28235,20 @@
         <v>105</v>
       </c>
       <c r="E704" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F704" t="s">
         <v>95</v>
       </c>
       <c r="G704">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bf9968cc511b92e99f89e9856bd38fb6.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8530ec1d1281da71f660df7c61571e38.html","web")</f>
         <v>0</v>
       </c>
       <c r="J704" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K704" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M704" t="s">
         <v>95</v>
@@ -28250,7 +28259,7 @@
         <v>1467</v>
       </c>
       <c r="B705" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C705" t="s">
         <v>55</v>
@@ -28259,20 +28268,20 @@
         <v>105</v>
       </c>
       <c r="E705" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F705" t="s">
         <v>95</v>
       </c>
       <c r="G705">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/64c745ab7c8597bb0afed2bafd12c20c.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bf9968cc511b92e99f89e9856bd38fb6.html","web")</f>
         <v>0</v>
       </c>
       <c r="J705" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K705" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M705" t="s">
         <v>95</v>
@@ -28283,7 +28292,7 @@
         <v>1467</v>
       </c>
       <c r="B706" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C706" t="s">
         <v>55</v>
@@ -28292,20 +28301,20 @@
         <v>105</v>
       </c>
       <c r="E706" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F706" t="s">
         <v>95</v>
       </c>
       <c r="G706">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cbe53c2-12cc-11e6-b2bc-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/64c745ab7c8597bb0afed2bafd12c20c.html","web")</f>
         <v>0</v>
       </c>
       <c r="J706" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K706" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M706" t="s">
         <v>95</v>
@@ -28316,7 +28325,7 @@
         <v>1467</v>
       </c>
       <c r="B707" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C707" t="s">
         <v>55</v>
@@ -28325,20 +28334,20 @@
         <v>105</v>
       </c>
       <c r="E707" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F707" t="s">
         <v>95</v>
       </c>
       <c r="G707">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d447c41b5f4e8c44f1fe64503cb4caa1.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cbe53c2-12cc-11e6-b2bc-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J707" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="K707" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M707" t="s">
         <v>95</v>
@@ -28349,7 +28358,7 @@
         <v>1467</v>
       </c>
       <c r="B708" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C708" t="s">
         <v>55</v>
@@ -28358,23 +28367,23 @@
         <v>105</v>
       </c>
       <c r="E708" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F708" t="s">
-        <v>202</v>
+        <v>95</v>
       </c>
       <c r="G708">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9259f1caedb47c287bc1c9dfc3c6f756.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d447c41b5f4e8c44f1fe64503cb4caa1.html","web")</f>
         <v>0</v>
       </c>
       <c r="J708" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K708" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M708" t="s">
-        <v>202</v>
+        <v>95</v>
       </c>
     </row>
     <row r="709" spans="1:13">
@@ -28382,32 +28391,32 @@
         <v>1467</v>
       </c>
       <c r="B709" t="s">
-        <v>1689</v>
+        <v>244</v>
       </c>
       <c r="C709" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D709" t="s">
         <v>105</v>
       </c>
       <c r="E709" t="s">
-        <v>1690</v>
+        <v>245</v>
       </c>
       <c r="F709" t="s">
-        <v>1691</v>
+        <v>202</v>
       </c>
       <c r="G709">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15410a16-f746-11e5-950e-5404a60d96b5.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9259f1caedb47c287bc1c9dfc3c6f756.html","web")</f>
         <v>0</v>
       </c>
       <c r="J709" t="s">
-        <v>1692</v>
+        <v>246</v>
       </c>
       <c r="K709" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="M709" t="s">
-        <v>1691</v>
+        <v>202</v>
       </c>
     </row>
     <row r="710" spans="1:13">
@@ -28415,32 +28424,32 @@
         <v>1467</v>
       </c>
       <c r="B710" t="s">
-        <v>1179</v>
+        <v>1692</v>
       </c>
       <c r="C710" t="s">
         <v>35</v>
       </c>
       <c r="D710" t="s">
-        <v>1383</v>
+        <v>105</v>
       </c>
       <c r="E710" t="s">
-        <v>1181</v>
+        <v>1693</v>
       </c>
       <c r="F710" t="s">
-        <v>35</v>
+        <v>1694</v>
       </c>
       <c r="G710">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a06b8e83250b870d9f39dc1f6534efcb.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15410a16-f746-11e5-950e-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="J710" t="s">
-        <v>1182</v>
+        <v>1695</v>
       </c>
       <c r="K710" t="s">
-        <v>346</v>
+        <v>1678</v>
       </c>
       <c r="M710" t="s">
-        <v>35</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="711" spans="1:13">
@@ -28448,32 +28457,32 @@
         <v>1467</v>
       </c>
       <c r="B711" t="s">
-        <v>1693</v>
+        <v>1179</v>
       </c>
       <c r="C711" t="s">
         <v>35</v>
       </c>
       <c r="D711" t="s">
-        <v>105</v>
+        <v>1383</v>
       </c>
       <c r="E711" t="s">
-        <v>1694</v>
+        <v>1181</v>
       </c>
       <c r="F711" t="s">
-        <v>1691</v>
+        <v>35</v>
       </c>
       <c r="G711">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590df00c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a06b8e83250b870d9f39dc1f6534efcb.html","web")</f>
         <v>0</v>
       </c>
       <c r="J711" t="s">
-        <v>1695</v>
+        <v>1182</v>
       </c>
       <c r="K711" t="s">
-        <v>1675</v>
+        <v>346</v>
       </c>
       <c r="M711" t="s">
-        <v>1691</v>
+        <v>35</v>
       </c>
     </row>
     <row r="712" spans="1:13">
@@ -28481,32 +28490,32 @@
         <v>1467</v>
       </c>
       <c r="B712" t="s">
-        <v>277</v>
+        <v>1696</v>
       </c>
       <c r="C712" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D712" t="s">
         <v>105</v>
       </c>
       <c r="E712" t="s">
-        <v>278</v>
+        <v>1697</v>
       </c>
       <c r="F712" t="s">
-        <v>115</v>
+        <v>1694</v>
       </c>
       <c r="G712">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e526caea-dd83-11e5-9194-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590df00c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J712" t="s">
-        <v>279</v>
+        <v>1698</v>
       </c>
       <c r="K712" t="s">
-        <v>1382</v>
+        <v>1678</v>
       </c>
       <c r="M712" t="s">
-        <v>115</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="713" spans="1:13">
@@ -28514,7 +28523,7 @@
         <v>1467</v>
       </c>
       <c r="B713" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C713" t="s">
         <v>16</v>
@@ -28523,17 +28532,17 @@
         <v>105</v>
       </c>
       <c r="E713" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F713" t="s">
         <v>115</v>
       </c>
       <c r="G713">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e52644bc-dd83-11e5-9194-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e526caea-dd83-11e5-9194-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J713" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K713" t="s">
         <v>1382</v>
@@ -28547,7 +28556,7 @@
         <v>1467</v>
       </c>
       <c r="B714" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C714" t="s">
         <v>16</v>
@@ -28556,17 +28565,17 @@
         <v>105</v>
       </c>
       <c r="E714" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F714" t="s">
         <v>115</v>
       </c>
       <c r="G714">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e527532a-dd83-11e5-9194-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e52644bc-dd83-11e5-9194-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J714" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="K714" t="s">
         <v>1382</v>
@@ -28580,32 +28589,32 @@
         <v>1467</v>
       </c>
       <c r="B715" t="s">
-        <v>1696</v>
+        <v>283</v>
       </c>
       <c r="C715" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D715" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="E715" t="s">
-        <v>1697</v>
+        <v>284</v>
       </c>
       <c r="F715" t="s">
-        <v>202</v>
+        <v>115</v>
       </c>
       <c r="G715">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f10b8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e527532a-dd83-11e5-9194-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J715" t="s">
-        <v>1698</v>
+        <v>285</v>
       </c>
       <c r="K715" t="s">
-        <v>1471</v>
+        <v>1382</v>
       </c>
       <c r="M715" t="s">
-        <v>202</v>
+        <v>115</v>
       </c>
     </row>
     <row r="716" spans="1:13">
@@ -28628,7 +28637,7 @@
         <v>202</v>
       </c>
       <c r="G716">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e4408-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f10b8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J716" t="s">
@@ -28661,7 +28670,7 @@
         <v>202</v>
       </c>
       <c r="G717">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e105a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e4408-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J717" t="s">
@@ -28685,26 +28694,26 @@
         <v>35</v>
       </c>
       <c r="D718" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="E718" t="s">
         <v>1706</v>
       </c>
       <c r="F718" t="s">
-        <v>1691</v>
+        <v>202</v>
       </c>
       <c r="G718">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/11806b1e-f747-11e5-950e-5404a60d96b5.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e105a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J718" t="s">
         <v>1707</v>
       </c>
       <c r="K718" t="s">
-        <v>1675</v>
+        <v>1471</v>
       </c>
       <c r="M718" t="s">
-        <v>1691</v>
+        <v>202</v>
       </c>
     </row>
     <row r="719" spans="1:13">
@@ -28712,32 +28721,32 @@
         <v>1467</v>
       </c>
       <c r="B719" t="s">
-        <v>1040</v>
+        <v>1708</v>
       </c>
       <c r="C719" t="s">
         <v>35</v>
       </c>
       <c r="D719" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="E719" t="s">
-        <v>1041</v>
+        <v>1709</v>
       </c>
       <c r="F719" t="s">
-        <v>202</v>
+        <v>1694</v>
       </c>
       <c r="G719">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7553003ead183dd3276108b6311a337f.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/11806b1e-f747-11e5-950e-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="J719" t="s">
-        <v>1042</v>
+        <v>1710</v>
       </c>
       <c r="K719" t="s">
-        <v>1043</v>
+        <v>1678</v>
       </c>
       <c r="M719" t="s">
-        <v>202</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="720" spans="1:13">
@@ -28745,7 +28754,7 @@
         <v>1467</v>
       </c>
       <c r="B720" t="s">
-        <v>1708</v>
+        <v>1040</v>
       </c>
       <c r="C720" t="s">
         <v>35</v>
@@ -28754,20 +28763,20 @@
         <v>172</v>
       </c>
       <c r="E720" t="s">
-        <v>1709</v>
+        <v>1041</v>
       </c>
       <c r="F720" t="s">
         <v>202</v>
       </c>
       <c r="G720">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591401a4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7553003ead183dd3276108b6311a337f.html","web")</f>
         <v>0</v>
       </c>
       <c r="J720" t="s">
-        <v>1710</v>
+        <v>1042</v>
       </c>
       <c r="K720" t="s">
-        <v>1471</v>
+        <v>1043</v>
       </c>
       <c r="M720" t="s">
         <v>202</v>
@@ -28793,7 +28802,7 @@
         <v>202</v>
       </c>
       <c r="G721">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591763b2-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591401a4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J721" t="s">
@@ -28826,7 +28835,7 @@
         <v>202</v>
       </c>
       <c r="G722">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912fb88-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591763b2-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J722" t="s">
@@ -28850,26 +28859,26 @@
         <v>35</v>
       </c>
       <c r="D723" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="E723" t="s">
         <v>1718</v>
       </c>
       <c r="F723" t="s">
-        <v>1691</v>
+        <v>202</v>
       </c>
       <c r="G723">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914af46-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912fb88-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J723" t="s">
         <v>1719</v>
       </c>
       <c r="K723" t="s">
-        <v>1675</v>
+        <v>1471</v>
       </c>
       <c r="M723" t="s">
-        <v>1691</v>
+        <v>202</v>
       </c>
     </row>
     <row r="724" spans="1:13">
@@ -28883,26 +28892,26 @@
         <v>35</v>
       </c>
       <c r="D724" t="s">
-        <v>619</v>
+        <v>105</v>
       </c>
       <c r="E724" t="s">
         <v>1721</v>
       </c>
       <c r="F724" t="s">
-        <v>50</v>
+        <v>1694</v>
       </c>
       <c r="G724">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f7e72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914af46-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J724" t="s">
         <v>1722</v>
       </c>
       <c r="K724" t="s">
-        <v>1471</v>
+        <v>1678</v>
       </c>
       <c r="M724" t="s">
-        <v>50</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="725" spans="1:13">
@@ -28916,7 +28925,7 @@
         <v>35</v>
       </c>
       <c r="D725" t="s">
-        <v>105</v>
+        <v>619</v>
       </c>
       <c r="E725" t="s">
         <v>1724</v>
@@ -28925,7 +28934,7 @@
         <v>50</v>
       </c>
       <c r="G725">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e0dd0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f7e72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J725" t="s">
@@ -28949,7 +28958,7 @@
         <v>35</v>
       </c>
       <c r="D726" t="s">
-        <v>619</v>
+        <v>105</v>
       </c>
       <c r="E726" t="s">
         <v>1727</v>
@@ -28958,7 +28967,7 @@
         <v>50</v>
       </c>
       <c r="G726">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914fd52-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e0dd0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J726" t="s">
@@ -28979,29 +28988,29 @@
         <v>1729</v>
       </c>
       <c r="C727" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D727" t="s">
-        <v>172</v>
+        <v>619</v>
       </c>
       <c r="E727" t="s">
         <v>1730</v>
       </c>
       <c r="F727" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
       <c r="G727">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f108a8-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914fd52-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J727" t="s">
         <v>1731</v>
       </c>
       <c r="K727" t="s">
-        <v>1500</v>
+        <v>1471</v>
       </c>
       <c r="M727" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
     </row>
     <row r="728" spans="1:13">
@@ -29024,14 +29033,14 @@
         <v>202</v>
       </c>
       <c r="G728">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590dd13a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f108a8-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J728" t="s">
         <v>1734</v>
       </c>
       <c r="K728" t="s">
-        <v>1475</v>
+        <v>1500</v>
       </c>
       <c r="M728" t="s">
         <v>202</v>
@@ -29057,7 +29066,7 @@
         <v>202</v>
       </c>
       <c r="G729">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914517c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590dd13a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J729" t="s">
@@ -29075,32 +29084,32 @@
         <v>1467</v>
       </c>
       <c r="B730" t="s">
-        <v>1322</v>
+        <v>1738</v>
       </c>
       <c r="C730" t="s">
         <v>55</v>
       </c>
       <c r="D730" t="s">
-        <v>1542</v>
+        <v>172</v>
       </c>
       <c r="E730" t="s">
-        <v>1323</v>
+        <v>1739</v>
       </c>
       <c r="F730" t="s">
-        <v>35</v>
+        <v>202</v>
       </c>
       <c r="G730">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914b9be-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914517c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J730" t="s">
-        <v>1324</v>
+        <v>1740</v>
       </c>
       <c r="K730" t="s">
-        <v>21</v>
+        <v>1475</v>
       </c>
       <c r="M730" t="s">
-        <v>35</v>
+        <v>202</v>
       </c>
     </row>
     <row r="731" spans="1:13">
@@ -29108,32 +29117,32 @@
         <v>1467</v>
       </c>
       <c r="B731" t="s">
-        <v>1229</v>
+        <v>1322</v>
       </c>
       <c r="C731" t="s">
         <v>55</v>
       </c>
       <c r="D731" t="s">
-        <v>619</v>
+        <v>1542</v>
       </c>
       <c r="E731" t="s">
-        <v>1230</v>
+        <v>1323</v>
       </c>
       <c r="F731" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="G731">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d80ff3a0dec0b1256a0943aadab66813.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914b9be-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J731" t="s">
-        <v>1231</v>
+        <v>1324</v>
       </c>
       <c r="K731" t="s">
-        <v>1152</v>
+        <v>21</v>
       </c>
       <c r="M731" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="732" spans="1:13">
@@ -29141,7 +29150,7 @@
         <v>1467</v>
       </c>
       <c r="B732" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="C732" t="s">
         <v>55</v>
@@ -29150,13 +29159,13 @@
         <v>619</v>
       </c>
       <c r="E732" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="F732" t="s">
         <v>69</v>
       </c>
       <c r="G732">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c2270065bb39bfa4fbf0d13a78dfa8a1.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d80ff3a0dec0b1256a0943aadab66813.html","web")</f>
         <v>0</v>
       </c>
       <c r="J732" t="s">
@@ -29174,7 +29183,7 @@
         <v>1467</v>
       </c>
       <c r="B733" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C733" t="s">
         <v>55</v>
@@ -29183,20 +29192,20 @@
         <v>619</v>
       </c>
       <c r="E733" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="F733" t="s">
         <v>69</v>
       </c>
       <c r="G733">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7aa8f285b17a5bcfce416f19c29d6d72.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c2270065bb39bfa4fbf0d13a78dfa8a1.html","web")</f>
         <v>0</v>
       </c>
       <c r="J733" t="s">
-        <v>1236</v>
+        <v>1231</v>
       </c>
       <c r="K733" t="s">
-        <v>1738</v>
+        <v>1152</v>
       </c>
       <c r="M733" t="s">
         <v>69</v>
@@ -29207,7 +29216,7 @@
         <v>1467</v>
       </c>
       <c r="B734" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="C734" t="s">
         <v>55</v>
@@ -29216,20 +29225,20 @@
         <v>619</v>
       </c>
       <c r="E734" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="F734" t="s">
         <v>69</v>
       </c>
       <c r="G734">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ed2fff61c68d8a09d5034168e82ae862.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7aa8f285b17a5bcfce416f19c29d6d72.html","web")</f>
         <v>0</v>
       </c>
       <c r="J734" t="s">
         <v>1236</v>
       </c>
       <c r="K734" t="s">
-        <v>1738</v>
+        <v>1741</v>
       </c>
       <c r="M734" t="s">
         <v>69</v>
@@ -29240,32 +29249,32 @@
         <v>1467</v>
       </c>
       <c r="B735" t="s">
-        <v>1739</v>
+        <v>1237</v>
       </c>
       <c r="C735" t="s">
         <v>55</v>
       </c>
       <c r="D735" t="s">
-        <v>172</v>
+        <v>619</v>
       </c>
       <c r="E735" t="s">
-        <v>1740</v>
+        <v>1238</v>
       </c>
       <c r="F735" t="s">
-        <v>202</v>
+        <v>69</v>
       </c>
       <c r="G735">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0beac-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ed2fff61c68d8a09d5034168e82ae862.html","web")</f>
         <v>0</v>
       </c>
       <c r="J735" t="s">
+        <v>1236</v>
+      </c>
+      <c r="K735" t="s">
         <v>1741</v>
       </c>
-      <c r="K735" t="s">
-        <v>1500</v>
-      </c>
       <c r="M735" t="s">
-        <v>202</v>
+        <v>69</v>
       </c>
     </row>
     <row r="736" spans="1:13">
@@ -29288,7 +29297,7 @@
         <v>202</v>
       </c>
       <c r="G736">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0f354-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0beac-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J736" t="s">
@@ -29321,7 +29330,7 @@
         <v>202</v>
       </c>
       <c r="G737">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f1117c-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0f354-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J737" t="s">
@@ -29354,14 +29363,14 @@
         <v>202</v>
       </c>
       <c r="G738">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f1f68-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f1117c-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J738" t="s">
         <v>1750</v>
       </c>
       <c r="K738" t="s">
-        <v>1475</v>
+        <v>1500</v>
       </c>
       <c r="M738" t="s">
         <v>202</v>
@@ -29387,11 +29396,11 @@
         <v>202</v>
       </c>
       <c r="G739">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f2436-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f1f68-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J739" t="s">
-        <v>1750</v>
+        <v>1753</v>
       </c>
       <c r="K739" t="s">
         <v>1475</v>
@@ -29405,32 +29414,32 @@
         <v>1467</v>
       </c>
       <c r="B740" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C740" t="s">
+        <v>55</v>
+      </c>
+      <c r="D740" t="s">
+        <v>172</v>
+      </c>
+      <c r="E740" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F740" t="s">
+        <v>202</v>
+      </c>
+      <c r="G740">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f2436-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J740" t="s">
         <v>1753</v>
       </c>
-      <c r="C740" t="s">
-        <v>35</v>
-      </c>
-      <c r="D740" t="s">
-        <v>1602</v>
-      </c>
-      <c r="E740" t="s">
-        <v>1754</v>
-      </c>
-      <c r="F740" t="s">
-        <v>95</v>
-      </c>
-      <c r="G740">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912c3de-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J740" t="s">
-        <v>1755</v>
-      </c>
       <c r="K740" t="s">
-        <v>1605</v>
+        <v>1475</v>
       </c>
       <c r="M740" t="s">
-        <v>95</v>
+        <v>202</v>
       </c>
     </row>
     <row r="741" spans="1:13">
@@ -29438,29 +29447,29 @@
         <v>1467</v>
       </c>
       <c r="B741" t="s">
-        <v>286</v>
+        <v>1756</v>
       </c>
       <c r="C741" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D741" t="s">
-        <v>105</v>
+        <v>1605</v>
       </c>
       <c r="E741" t="s">
-        <v>287</v>
+        <v>1757</v>
       </c>
       <c r="F741" t="s">
         <v>95</v>
       </c>
       <c r="G741">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b2f82090-fbed-11e5-8f03-5404a60d96b5.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912c3de-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J741" t="s">
-        <v>288</v>
+        <v>1758</v>
       </c>
       <c r="K741" t="s">
-        <v>1675</v>
+        <v>1608</v>
       </c>
       <c r="M741" t="s">
         <v>95</v>
@@ -29471,29 +29480,29 @@
         <v>1467</v>
       </c>
       <c r="B742" t="s">
-        <v>1391</v>
+        <v>286</v>
       </c>
       <c r="C742" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D742" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="E742" t="s">
-        <v>1392</v>
+        <v>287</v>
       </c>
       <c r="F742" t="s">
         <v>95</v>
       </c>
       <c r="G742">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6ca9dd8a089b15fb96841e9fe56411cf.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b2f82090-fbed-11e5-8f03-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="J742" t="s">
-        <v>1393</v>
+        <v>288</v>
       </c>
       <c r="K742" t="s">
-        <v>1547</v>
+        <v>1678</v>
       </c>
       <c r="M742" t="s">
         <v>95</v>
@@ -29504,7 +29513,7 @@
         <v>1467</v>
       </c>
       <c r="B743" t="s">
-        <v>549</v>
+        <v>1391</v>
       </c>
       <c r="C743" t="s">
         <v>35</v>
@@ -29513,17 +29522,17 @@
         <v>172</v>
       </c>
       <c r="E743" t="s">
-        <v>550</v>
+        <v>1392</v>
       </c>
       <c r="F743" t="s">
         <v>95</v>
       </c>
       <c r="G743">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6ca9dd8a089b15fb96841e9fe56411cf.html","web")</f>
         <v>0</v>
       </c>
       <c r="J743" t="s">
-        <v>551</v>
+        <v>1393</v>
       </c>
       <c r="K743" t="s">
         <v>1547</v>
@@ -29537,29 +29546,29 @@
         <v>1467</v>
       </c>
       <c r="B744" t="s">
-        <v>1756</v>
+        <v>549</v>
       </c>
       <c r="C744" t="s">
         <v>35</v>
       </c>
       <c r="D744" t="s">
-        <v>1602</v>
+        <v>172</v>
       </c>
       <c r="E744" t="s">
-        <v>1757</v>
+        <v>550</v>
       </c>
       <c r="F744" t="s">
         <v>95</v>
       </c>
       <c r="G744">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912e6d4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
         <v>0</v>
       </c>
       <c r="J744" t="s">
-        <v>1758</v>
+        <v>551</v>
       </c>
       <c r="K744" t="s">
-        <v>1605</v>
+        <v>1547</v>
       </c>
       <c r="M744" t="s">
         <v>95</v>
@@ -29576,26 +29585,26 @@
         <v>35</v>
       </c>
       <c r="D745" t="s">
-        <v>172</v>
+        <v>1605</v>
       </c>
       <c r="E745" t="s">
         <v>1760</v>
       </c>
       <c r="F745" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="G745">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1ca290c839426f31f70a0d2862e1c611.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912e6d4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J745" t="s">
         <v>1761</v>
       </c>
       <c r="K745" t="s">
-        <v>1543</v>
+        <v>1608</v>
       </c>
       <c r="M745" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="746" spans="1:13">
@@ -29618,7 +29627,7 @@
         <v>135</v>
       </c>
       <c r="G746">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/96435c8c0c0a8a7423d6abb6c027da69.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1ca290c839426f31f70a0d2862e1c611.html","web")</f>
         <v>0</v>
       </c>
       <c r="J746" t="s">
@@ -29651,14 +29660,14 @@
         <v>135</v>
       </c>
       <c r="G747">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/31a3caf70db7a8ed71e8d0a226365105.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/96435c8c0c0a8a7423d6abb6c027da69.html","web")</f>
         <v>0</v>
       </c>
       <c r="J747" t="s">
         <v>1767</v>
       </c>
       <c r="K747" t="s">
-        <v>1547</v>
+        <v>1543</v>
       </c>
       <c r="M747" t="s">
         <v>135</v>
@@ -29669,32 +29678,32 @@
         <v>1467</v>
       </c>
       <c r="B748" t="s">
-        <v>1325</v>
+        <v>1768</v>
       </c>
       <c r="C748" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D748" t="s">
-        <v>1542</v>
+        <v>172</v>
       </c>
       <c r="E748" t="s">
-        <v>1326</v>
+        <v>1769</v>
       </c>
       <c r="F748" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="G748">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917d1d0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/31a3caf70db7a8ed71e8d0a226365105.html","web")</f>
         <v>0</v>
       </c>
       <c r="J748" t="s">
-        <v>1327</v>
+        <v>1770</v>
       </c>
       <c r="K748" t="s">
-        <v>21</v>
+        <v>1547</v>
       </c>
       <c r="M748" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
     </row>
     <row r="749" spans="1:13">
@@ -29702,29 +29711,29 @@
         <v>1467</v>
       </c>
       <c r="B749" t="s">
-        <v>1768</v>
+        <v>1325</v>
       </c>
       <c r="C749" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D749" t="s">
-        <v>105</v>
+        <v>1542</v>
       </c>
       <c r="E749" t="s">
-        <v>1769</v>
+        <v>1326</v>
       </c>
       <c r="F749" t="s">
         <v>35</v>
       </c>
       <c r="G749">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cbf-4d35-11e8-be0a-1c4d70487308.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917d1d0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J749" t="s">
-        <v>1770</v>
+        <v>1327</v>
       </c>
       <c r="K749" t="s">
-        <v>1471</v>
+        <v>21</v>
       </c>
       <c r="M749" t="s">
         <v>35</v>
@@ -29750,7 +29759,7 @@
         <v>35</v>
       </c>
       <c r="G750">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cc0-4d35-11e8-be0a-1c4d70487308.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cbf-4d35-11e8-be0a-1c4d70487308.html","web")</f>
         <v>0</v>
       </c>
       <c r="J750" t="s">
@@ -29774,26 +29783,26 @@
         <v>35</v>
       </c>
       <c r="D751" t="s">
-        <v>1602</v>
+        <v>105</v>
       </c>
       <c r="E751" t="s">
         <v>1775</v>
       </c>
       <c r="F751" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="G751">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e379c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fdca5cc0-4d35-11e8-be0a-1c4d70487308.html","web")</f>
         <v>0</v>
       </c>
       <c r="J751" t="s">
         <v>1776</v>
       </c>
       <c r="K751" t="s">
-        <v>1605</v>
+        <v>1471</v>
       </c>
       <c r="M751" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="752" spans="1:13">
@@ -29807,26 +29816,26 @@
         <v>35</v>
       </c>
       <c r="D752" t="s">
-        <v>172</v>
+        <v>1605</v>
       </c>
       <c r="E752" t="s">
         <v>1778</v>
       </c>
       <c r="F752" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="G752">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f465a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e379c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J752" t="s">
-        <v>1644</v>
+        <v>1779</v>
       </c>
       <c r="K752" t="s">
-        <v>1471</v>
+        <v>1608</v>
       </c>
       <c r="M752" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="753" spans="1:13">
@@ -29834,7 +29843,7 @@
         <v>1467</v>
       </c>
       <c r="B753" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="C753" t="s">
         <v>35</v>
@@ -29843,17 +29852,17 @@
         <v>172</v>
       </c>
       <c r="E753" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="F753" t="s">
         <v>95</v>
       </c>
       <c r="G753">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917cf46-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f465a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J753" t="s">
-        <v>1781</v>
+        <v>1647</v>
       </c>
       <c r="K753" t="s">
         <v>1471</v>
@@ -29882,11 +29891,11 @@
         <v>95</v>
       </c>
       <c r="G754">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4cabf9607859a83bcb3bc00fa8d0698c.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917cf46-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J754" t="s">
-        <v>1650</v>
+        <v>1784</v>
       </c>
       <c r="K754" t="s">
         <v>1471</v>
@@ -29900,7 +29909,7 @@
         <v>1467</v>
       </c>
       <c r="B755" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="C755" t="s">
         <v>35</v>
@@ -29909,17 +29918,17 @@
         <v>172</v>
       </c>
       <c r="E755" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="F755" t="s">
         <v>95</v>
       </c>
       <c r="G755">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/332db812bf06c7af2de1b9d1e0cf58c9.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4cabf9607859a83bcb3bc00fa8d0698c.html","web")</f>
         <v>0</v>
       </c>
       <c r="J755" t="s">
-        <v>1650</v>
+        <v>1653</v>
       </c>
       <c r="K755" t="s">
         <v>1471</v>
@@ -29933,32 +29942,32 @@
         <v>1467</v>
       </c>
       <c r="B756" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
       <c r="C756" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D756" t="s">
-        <v>1520</v>
+        <v>172</v>
       </c>
       <c r="E756" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="F756" t="s">
-        <v>518</v>
+        <v>95</v>
       </c>
       <c r="G756">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f1146a-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/332db812bf06c7af2de1b9d1e0cf58c9.html","web")</f>
         <v>0</v>
       </c>
       <c r="J756" t="s">
-        <v>1788</v>
+        <v>1653</v>
       </c>
       <c r="K756" t="s">
-        <v>1500</v>
+        <v>1471</v>
       </c>
       <c r="M756" t="s">
-        <v>518</v>
+        <v>95</v>
       </c>
     </row>
     <row r="757" spans="1:13">
@@ -29969,29 +29978,29 @@
         <v>1789</v>
       </c>
       <c r="C757" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D757" t="s">
-        <v>1625</v>
+        <v>1520</v>
       </c>
       <c r="E757" t="s">
         <v>1790</v>
       </c>
       <c r="F757" t="s">
-        <v>325</v>
+        <v>518</v>
       </c>
       <c r="G757">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f1a90-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f1146a-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J757" t="s">
         <v>1791</v>
       </c>
       <c r="K757" t="s">
-        <v>1605</v>
+        <v>1500</v>
       </c>
       <c r="M757" t="s">
-        <v>325</v>
+        <v>518</v>
       </c>
     </row>
     <row r="758" spans="1:13">
@@ -29999,29 +30008,29 @@
         <v>1467</v>
       </c>
       <c r="B758" t="s">
-        <v>1397</v>
+        <v>1792</v>
       </c>
       <c r="C758" t="s">
         <v>35</v>
       </c>
       <c r="D758" t="s">
-        <v>1349</v>
+        <v>1628</v>
       </c>
       <c r="E758" t="s">
-        <v>1398</v>
+        <v>1793</v>
       </c>
       <c r="F758" t="s">
         <v>325</v>
       </c>
       <c r="G758">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/170ff384-b622-11e6-bbe2-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f1a90-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J758" t="s">
-        <v>1399</v>
+        <v>1794</v>
       </c>
       <c r="K758" t="s">
-        <v>1048</v>
+        <v>1608</v>
       </c>
       <c r="M758" t="s">
         <v>325</v>
@@ -30032,7 +30041,7 @@
         <v>1467</v>
       </c>
       <c r="B759" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="C759" t="s">
         <v>35</v>
@@ -30041,17 +30050,17 @@
         <v>1349</v>
       </c>
       <c r="E759" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="F759" t="s">
         <v>325</v>
       </c>
       <c r="G759">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1758307c-b622-11e6-bbe2-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/170ff384-b622-11e6-bbe2-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J759" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="K759" t="s">
         <v>1048</v>
@@ -30065,32 +30074,32 @@
         <v>1467</v>
       </c>
       <c r="B760" t="s">
-        <v>1239</v>
+        <v>1400</v>
       </c>
       <c r="C760" t="s">
         <v>35</v>
       </c>
       <c r="D760" t="s">
-        <v>619</v>
+        <v>1349</v>
       </c>
       <c r="E760" t="s">
-        <v>1240</v>
+        <v>1401</v>
       </c>
       <c r="F760" t="s">
-        <v>518</v>
+        <v>325</v>
       </c>
       <c r="G760">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ec6bc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1758307c-b622-11e6-bbe2-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J760" t="s">
-        <v>1241</v>
+        <v>1402</v>
       </c>
       <c r="K760" t="s">
-        <v>1152</v>
+        <v>1048</v>
       </c>
       <c r="M760" t="s">
-        <v>518</v>
+        <v>325</v>
       </c>
     </row>
     <row r="761" spans="1:13">
@@ -30098,7 +30107,7 @@
         <v>1467</v>
       </c>
       <c r="B761" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="C761" t="s">
         <v>35</v>
@@ -30107,17 +30116,17 @@
         <v>619</v>
       </c>
       <c r="E761" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="F761" t="s">
         <v>518</v>
       </c>
       <c r="G761">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59135d8a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ec6bc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J761" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="K761" t="s">
         <v>1152</v>
@@ -30131,7 +30140,7 @@
         <v>1467</v>
       </c>
       <c r="B762" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="C762" t="s">
         <v>35</v>
@@ -30140,23 +30149,23 @@
         <v>619</v>
       </c>
       <c r="E762" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="F762" t="s">
-        <v>19</v>
+        <v>518</v>
       </c>
       <c r="G762">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590dcb0e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59135d8a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J762" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="K762" t="s">
         <v>1152</v>
       </c>
       <c r="M762" t="s">
-        <v>19</v>
+        <v>518</v>
       </c>
     </row>
     <row r="763" spans="1:13">
@@ -30164,29 +30173,29 @@
         <v>1467</v>
       </c>
       <c r="B763" t="s">
-        <v>1792</v>
+        <v>1245</v>
       </c>
       <c r="C763" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D763" t="s">
-        <v>1542</v>
+        <v>619</v>
       </c>
       <c r="E763" t="s">
-        <v>542</v>
+        <v>1246</v>
       </c>
       <c r="F763" t="s">
         <v>19</v>
       </c>
       <c r="G763">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/621681bc7c376de66228fdde13b97516.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590dcb0e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J763" t="s">
-        <v>543</v>
+        <v>1247</v>
       </c>
       <c r="K763" t="s">
-        <v>21</v>
+        <v>1152</v>
       </c>
       <c r="M763" t="s">
         <v>19</v>
@@ -30197,29 +30206,29 @@
         <v>1467</v>
       </c>
       <c r="B764" t="s">
-        <v>1248</v>
+        <v>1795</v>
       </c>
       <c r="C764" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D764" t="s">
-        <v>619</v>
+        <v>1542</v>
       </c>
       <c r="E764" t="s">
-        <v>1249</v>
+        <v>542</v>
       </c>
       <c r="F764" t="s">
         <v>19</v>
       </c>
       <c r="G764">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59143570-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/621681bc7c376de66228fdde13b97516.html","web")</f>
         <v>0</v>
       </c>
       <c r="J764" t="s">
-        <v>1241</v>
+        <v>543</v>
       </c>
       <c r="K764" t="s">
-        <v>1152</v>
+        <v>21</v>
       </c>
       <c r="M764" t="s">
         <v>19</v>
@@ -30230,29 +30239,29 @@
         <v>1467</v>
       </c>
       <c r="B765" t="s">
-        <v>1793</v>
+        <v>1248</v>
       </c>
       <c r="C765" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D765" t="s">
-        <v>1542</v>
+        <v>619</v>
       </c>
       <c r="E765" t="s">
-        <v>967</v>
+        <v>1249</v>
       </c>
       <c r="F765" t="s">
         <v>19</v>
       </c>
       <c r="G765">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917483c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59143570-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J765" t="s">
-        <v>968</v>
+        <v>1241</v>
       </c>
       <c r="K765" t="s">
-        <v>21</v>
+        <v>1152</v>
       </c>
       <c r="M765" t="s">
         <v>19</v>
@@ -30263,29 +30272,29 @@
         <v>1467</v>
       </c>
       <c r="B766" t="s">
-        <v>969</v>
+        <v>1796</v>
       </c>
       <c r="C766" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D766" t="s">
-        <v>619</v>
+        <v>1542</v>
       </c>
       <c r="E766" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="F766" t="s">
         <v>19</v>
       </c>
       <c r="G766">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59170a02-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917483c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J766" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="K766" t="s">
-        <v>1152</v>
+        <v>21</v>
       </c>
       <c r="M766" t="s">
         <v>19</v>
@@ -30296,29 +30305,29 @@
         <v>1467</v>
       </c>
       <c r="B767" t="s">
-        <v>1794</v>
+        <v>969</v>
       </c>
       <c r="C767" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D767" t="s">
-        <v>1542</v>
+        <v>619</v>
       </c>
       <c r="E767" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="F767" t="s">
         <v>19</v>
       </c>
       <c r="G767">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59173c0c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59170a02-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J767" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="K767" t="s">
-        <v>21</v>
+        <v>1152</v>
       </c>
       <c r="M767" t="s">
         <v>19</v>
@@ -30329,29 +30338,29 @@
         <v>1467</v>
       </c>
       <c r="B768" t="s">
-        <v>975</v>
+        <v>1797</v>
       </c>
       <c r="C768" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D768" t="s">
-        <v>619</v>
+        <v>1542</v>
       </c>
       <c r="E768" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="F768" t="s">
         <v>19</v>
       </c>
       <c r="G768">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913d86e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59173c0c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J768" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="K768" t="s">
-        <v>1152</v>
+        <v>21</v>
       </c>
       <c r="M768" t="s">
         <v>19</v>
@@ -30362,7 +30371,7 @@
         <v>1467</v>
       </c>
       <c r="B769" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C769" t="s">
         <v>35</v>
@@ -30371,17 +30380,17 @@
         <v>619</v>
       </c>
       <c r="E769" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="F769" t="s">
         <v>19</v>
       </c>
       <c r="G769">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913d602-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913d86e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J769" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="K769" t="s">
         <v>1152</v>
@@ -30395,32 +30404,32 @@
         <v>1467</v>
       </c>
       <c r="B770" t="s">
-        <v>1795</v>
+        <v>978</v>
       </c>
       <c r="C770" t="s">
         <v>35</v>
       </c>
       <c r="D770" t="s">
-        <v>1602</v>
+        <v>619</v>
       </c>
       <c r="E770" t="s">
-        <v>1796</v>
+        <v>979</v>
       </c>
       <c r="F770" t="s">
-        <v>325</v>
+        <v>19</v>
       </c>
       <c r="G770">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e417e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913d602-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J770" t="s">
-        <v>1797</v>
+        <v>980</v>
       </c>
       <c r="K770" t="s">
-        <v>1605</v>
+        <v>1152</v>
       </c>
       <c r="M770" t="s">
-        <v>325</v>
+        <v>19</v>
       </c>
     </row>
     <row r="771" spans="1:13">
@@ -30434,26 +30443,26 @@
         <v>35</v>
       </c>
       <c r="D771" t="s">
-        <v>172</v>
+        <v>1605</v>
       </c>
       <c r="E771" t="s">
         <v>1799</v>
       </c>
       <c r="F771" t="s">
-        <v>163</v>
+        <v>325</v>
       </c>
       <c r="G771">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e417e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J771" t="s">
         <v>1800</v>
       </c>
       <c r="K771" t="s">
-        <v>21</v>
+        <v>1608</v>
       </c>
       <c r="M771" t="s">
-        <v>163</v>
+        <v>325</v>
       </c>
     </row>
     <row r="772" spans="1:13">
@@ -30461,32 +30470,32 @@
         <v>1467</v>
       </c>
       <c r="B772" t="s">
-        <v>409</v>
+        <v>1801</v>
       </c>
       <c r="C772" t="s">
         <v>35</v>
       </c>
       <c r="D772" t="s">
-        <v>1011</v>
+        <v>172</v>
       </c>
       <c r="E772" t="s">
-        <v>23</v>
+        <v>1802</v>
       </c>
       <c r="F772" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="G772">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e85a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59177dc0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J772" t="s">
-        <v>25</v>
+        <v>1803</v>
       </c>
       <c r="K772" t="s">
-        <v>1801</v>
+        <v>21</v>
       </c>
       <c r="M772" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
     </row>
     <row r="773" spans="1:13">
@@ -30494,7 +30503,7 @@
         <v>1467</v>
       </c>
       <c r="B773" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C773" t="s">
         <v>35</v>
@@ -30503,20 +30512,20 @@
         <v>1011</v>
       </c>
       <c r="E773" t="s">
-        <v>411</v>
+        <v>23</v>
       </c>
       <c r="F773" t="s">
         <v>24</v>
       </c>
       <c r="G773">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ed5a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e85a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J773" t="s">
-        <v>412</v>
+        <v>25</v>
       </c>
       <c r="K773" t="s">
-        <v>1801</v>
+        <v>1804</v>
       </c>
       <c r="M773" t="s">
         <v>24</v>
@@ -30527,32 +30536,32 @@
         <v>1467</v>
       </c>
       <c r="B774" t="s">
-        <v>71</v>
+        <v>410</v>
       </c>
       <c r="C774" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D774" t="s">
-        <v>172</v>
+        <v>1011</v>
       </c>
       <c r="E774" t="s">
-        <v>73</v>
+        <v>411</v>
       </c>
       <c r="F774" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="G774">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59170cbe-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ed5a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J774" t="s">
-        <v>74</v>
+        <v>412</v>
       </c>
       <c r="K774" t="s">
-        <v>1802</v>
+        <v>1804</v>
       </c>
       <c r="M774" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="775" spans="1:13">
@@ -30560,7 +30569,7 @@
         <v>1467</v>
       </c>
       <c r="B775" t="s">
-        <v>1803</v>
+        <v>71</v>
       </c>
       <c r="C775" t="s">
         <v>55</v>
@@ -30569,20 +30578,20 @@
         <v>172</v>
       </c>
       <c r="E775" t="s">
-        <v>1804</v>
+        <v>73</v>
       </c>
       <c r="F775" t="s">
         <v>69</v>
       </c>
       <c r="G775">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917d9fa-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59170cbe-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J775" t="s">
+        <v>74</v>
+      </c>
+      <c r="K775" t="s">
         <v>1805</v>
-      </c>
-      <c r="K775" t="s">
-        <v>1475</v>
       </c>
       <c r="M775" t="s">
         <v>69</v>
@@ -30608,7 +30617,7 @@
         <v>69</v>
       </c>
       <c r="G776">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591384a4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917d9fa-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J776" t="s">
@@ -30641,14 +30650,14 @@
         <v>69</v>
       </c>
       <c r="G777">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0430a-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591384a4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J777" t="s">
         <v>1811</v>
       </c>
       <c r="K777" t="s">
-        <v>1500</v>
+        <v>1475</v>
       </c>
       <c r="M777" t="s">
         <v>69</v>
@@ -30674,14 +30683,14 @@
         <v>69</v>
       </c>
       <c r="G778">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59174aa8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/84f0430a-acb7-11e6-b5ee-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J778" t="s">
         <v>1814</v>
       </c>
       <c r="K778" t="s">
-        <v>1475</v>
+        <v>1500</v>
       </c>
       <c r="M778" t="s">
         <v>69</v>
@@ -30695,7 +30704,7 @@
         <v>1815</v>
       </c>
       <c r="C779" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D779" t="s">
         <v>172</v>
@@ -30704,20 +30713,20 @@
         <v>1816</v>
       </c>
       <c r="F779" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="G779">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59174aa8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J779" t="s">
         <v>1817</v>
       </c>
       <c r="K779" t="s">
-        <v>21</v>
+        <v>1475</v>
       </c>
       <c r="M779" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
     </row>
     <row r="780" spans="1:13">
@@ -30725,32 +30734,32 @@
         <v>1467</v>
       </c>
       <c r="B780" t="s">
-        <v>985</v>
+        <v>1818</v>
       </c>
       <c r="C780" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D780" t="s">
-        <v>1011</v>
+        <v>172</v>
       </c>
       <c r="E780" t="s">
-        <v>27</v>
+        <v>1819</v>
       </c>
       <c r="F780" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="G780">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59170700-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591306a0-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J780" t="s">
-        <v>28</v>
+        <v>1820</v>
       </c>
       <c r="K780" t="s">
-        <v>959</v>
+        <v>21</v>
       </c>
       <c r="M780" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
     </row>
     <row r="781" spans="1:13">
@@ -30758,7 +30767,7 @@
         <v>1467</v>
       </c>
       <c r="B781" t="s">
-        <v>1818</v>
+        <v>985</v>
       </c>
       <c r="C781" t="s">
         <v>55</v>
@@ -30767,17 +30776,17 @@
         <v>1011</v>
       </c>
       <c r="E781" t="s">
-        <v>1819</v>
+        <v>27</v>
       </c>
       <c r="F781" t="s">
         <v>24</v>
       </c>
       <c r="G781">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59140c12-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59170700-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J781" t="s">
-        <v>1820</v>
+        <v>28</v>
       </c>
       <c r="K781" t="s">
         <v>959</v>
@@ -30797,26 +30806,26 @@
         <v>55</v>
       </c>
       <c r="D782" t="s">
-        <v>172</v>
+        <v>1011</v>
       </c>
       <c r="E782" t="s">
         <v>1822</v>
       </c>
       <c r="F782" t="s">
-        <v>202</v>
+        <v>24</v>
       </c>
       <c r="G782">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a070-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59140c12-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J782" t="s">
         <v>1823</v>
       </c>
       <c r="K782" t="s">
-        <v>1475</v>
+        <v>959</v>
       </c>
       <c r="M782" t="s">
-        <v>202</v>
+        <v>24</v>
       </c>
     </row>
     <row r="783" spans="1:13">
@@ -30839,14 +30848,14 @@
         <v>202</v>
       </c>
       <c r="G783">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ec93c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a070-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J783" t="s">
         <v>1826</v>
       </c>
       <c r="K783" t="s">
-        <v>1500</v>
+        <v>1475</v>
       </c>
       <c r="M783" t="s">
         <v>202</v>
@@ -30872,7 +30881,7 @@
         <v>202</v>
       </c>
       <c r="G784">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f8fca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ec93c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J784" t="s">
@@ -30896,26 +30905,26 @@
         <v>55</v>
       </c>
       <c r="D785" t="s">
+        <v>172</v>
+      </c>
+      <c r="E785" t="s">
         <v>1831</v>
       </c>
-      <c r="E785" t="s">
+      <c r="F785" t="s">
+        <v>202</v>
+      </c>
+      <c r="G785">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f8fca-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J785" t="s">
         <v>1832</v>
       </c>
-      <c r="F785" t="s">
-        <v>42</v>
-      </c>
-      <c r="G785">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147ddc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J785" t="s">
-        <v>1833</v>
-      </c>
       <c r="K785" t="s">
-        <v>1834</v>
+        <v>1500</v>
       </c>
       <c r="M785" t="s">
-        <v>42</v>
+        <v>202</v>
       </c>
     </row>
     <row r="786" spans="1:13">
@@ -30923,32 +30932,32 @@
         <v>1467</v>
       </c>
       <c r="B786" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="C786" t="s">
         <v>55</v>
       </c>
       <c r="D786" t="s">
-        <v>172</v>
+        <v>1834</v>
       </c>
       <c r="E786" t="s">
+        <v>1835</v>
+      </c>
+      <c r="F786" t="s">
+        <v>42</v>
+      </c>
+      <c r="G786">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147ddc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J786" t="s">
         <v>1836</v>
       </c>
-      <c r="F786" t="s">
-        <v>69</v>
-      </c>
-      <c r="G786">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913c4dc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J786" t="s">
+      <c r="K786" t="s">
         <v>1837</v>
       </c>
-      <c r="K786" t="s">
-        <v>1500</v>
-      </c>
       <c r="M786" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="787" spans="1:13">
@@ -30956,32 +30965,32 @@
         <v>1467</v>
       </c>
       <c r="B787" t="s">
-        <v>986</v>
+        <v>1838</v>
       </c>
       <c r="C787" t="s">
         <v>55</v>
       </c>
       <c r="D787" t="s">
-        <v>619</v>
+        <v>172</v>
       </c>
       <c r="E787" t="s">
-        <v>987</v>
+        <v>1839</v>
       </c>
       <c r="F787" t="s">
-        <v>349</v>
+        <v>69</v>
       </c>
       <c r="G787">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591472f6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913c4dc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J787" t="s">
-        <v>988</v>
+        <v>1840</v>
       </c>
       <c r="K787" t="s">
-        <v>21</v>
+        <v>1500</v>
       </c>
       <c r="M787" t="s">
-        <v>349</v>
+        <v>69</v>
       </c>
     </row>
     <row r="788" spans="1:13">
@@ -30989,7 +30998,7 @@
         <v>1467</v>
       </c>
       <c r="B788" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="C788" t="s">
         <v>55</v>
@@ -30998,17 +31007,17 @@
         <v>619</v>
       </c>
       <c r="E788" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="F788" t="s">
         <v>349</v>
       </c>
       <c r="G788">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59132e1e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591472f6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J788" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="K788" t="s">
         <v>21</v>
@@ -31017,64 +31026,64 @@
         <v>349</v>
       </c>
     </row>
-    <row r="790" spans="1:13">
-      <c r="A790" t="s">
-        <v>1838</v>
-      </c>
-      <c r="B790" t="s">
-        <v>304</v>
-      </c>
-      <c r="C790" t="s">
+    <row r="789" spans="1:13">
+      <c r="A789" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B789" t="s">
+        <v>989</v>
+      </c>
+      <c r="C789" t="s">
         <v>55</v>
       </c>
-      <c r="D790" t="s">
-        <v>1839</v>
-      </c>
-      <c r="E790" t="s">
-        <v>306</v>
-      </c>
-      <c r="F790" t="s">
-        <v>202</v>
-      </c>
-      <c r="G790">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147580-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J790" t="s">
-        <v>307</v>
-      </c>
-      <c r="K790" t="s">
-        <v>91</v>
-      </c>
-      <c r="M790" t="s">
-        <v>202</v>
+      <c r="D789" t="s">
+        <v>619</v>
+      </c>
+      <c r="E789" t="s">
+        <v>990</v>
+      </c>
+      <c r="F789" t="s">
+        <v>349</v>
+      </c>
+      <c r="G789">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59132e1e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J789" t="s">
+        <v>991</v>
+      </c>
+      <c r="K789" t="s">
+        <v>21</v>
+      </c>
+      <c r="M789" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="791" spans="1:13">
       <c r="A791" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B791" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C791" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D791" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E791" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F791" t="s">
         <v>202</v>
       </c>
       <c r="G791">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e1c1c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147580-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J791" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="K791" t="s">
         <v>91</v>
@@ -31085,29 +31094,29 @@
     </row>
     <row r="792" spans="1:13">
       <c r="A792" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B792" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C792" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D792" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E792" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F792" t="s">
         <v>202</v>
       </c>
       <c r="G792">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41460524-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e1c1c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J792" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="K792" t="s">
         <v>91</v>
@@ -31118,29 +31127,29 @@
     </row>
     <row r="793" spans="1:13">
       <c r="A793" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B793" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C793" t="s">
         <v>55</v>
       </c>
       <c r="D793" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E793" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F793" t="s">
         <v>202</v>
       </c>
       <c r="G793">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4145ad04-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41460524-4f40-11e6-a814-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J793" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="K793" t="s">
         <v>91</v>
@@ -31151,29 +31160,29 @@
     </row>
     <row r="794" spans="1:13">
       <c r="A794" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B794" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C794" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D794" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E794" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F794" t="s">
         <v>202</v>
       </c>
       <c r="G794">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e4e58-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4145ad04-4f40-11e6-a814-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J794" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="K794" t="s">
         <v>91</v>
@@ -31184,29 +31193,29 @@
     </row>
     <row r="795" spans="1:13">
       <c r="A795" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B795" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C795" t="s">
         <v>16</v>
       </c>
       <c r="D795" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E795" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F795" t="s">
         <v>202</v>
       </c>
       <c r="G795">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59130394-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e4e58-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J795" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="K795" t="s">
         <v>91</v>
@@ -31217,62 +31226,62 @@
     </row>
     <row r="796" spans="1:13">
       <c r="A796" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B796" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C796" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="D796" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E796" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F796" t="s">
-        <v>325</v>
+        <v>202</v>
       </c>
       <c r="G796">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4144f026-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59130394-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J796" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="K796" t="s">
         <v>91</v>
       </c>
       <c r="M796" t="s">
-        <v>325</v>
+        <v>202</v>
       </c>
     </row>
     <row r="797" spans="1:13">
       <c r="A797" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B797" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C797" t="s">
         <v>55</v>
       </c>
       <c r="D797" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E797" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F797" t="s">
         <v>325</v>
       </c>
       <c r="G797">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4144a01c-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4144f026-4f40-11e6-a814-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J797" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="K797" t="s">
         <v>91</v>
@@ -31283,29 +31292,29 @@
     </row>
     <row r="798" spans="1:13">
       <c r="A798" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B798" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C798" t="s">
         <v>55</v>
       </c>
       <c r="D798" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E798" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F798" t="s">
         <v>325</v>
       </c>
       <c r="G798">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/14277100-b574-11e6-9ed4-5404a60d96b5.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4144a01c-4f40-11e6-a814-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J798" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K798" t="s">
         <v>91</v>
@@ -31316,62 +31325,62 @@
     </row>
     <row r="799" spans="1:13">
       <c r="A799" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B799" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C799" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D799" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E799" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F799" t="s">
-        <v>202</v>
+        <v>325</v>
       </c>
       <c r="G799">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/14277100-b574-11e6-9ed4-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="J799" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K799" t="s">
         <v>91</v>
       </c>
       <c r="M799" t="s">
-        <v>202</v>
+        <v>325</v>
       </c>
     </row>
     <row r="800" spans="1:13">
       <c r="A800" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B800" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C800" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D800" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E800" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F800" t="s">
         <v>202</v>
       </c>
       <c r="G800">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59150216-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/41455e80-4f40-11e6-a814-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="J800" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="K800" t="s">
         <v>91</v>
@@ -31382,29 +31391,29 @@
     </row>
     <row r="801" spans="1:13">
       <c r="A801" t="s">
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="B801" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C801" t="s">
         <v>55</v>
       </c>
       <c r="D801" t="s">
-        <v>1839</v>
+        <v>1842</v>
       </c>
       <c r="E801" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F801" t="s">
         <v>202</v>
       </c>
       <c r="G801">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912a516-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59150216-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J801" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="K801" t="s">
         <v>91</v>
@@ -31413,67 +31422,67 @@
         <v>202</v>
       </c>
     </row>
-    <row r="803" spans="1:13">
-      <c r="A803" t="s">
-        <v>1840</v>
-      </c>
-      <c r="B803" t="s">
+    <row r="802" spans="1:13">
+      <c r="A802" t="s">
         <v>1841</v>
       </c>
-      <c r="C803" t="s">
-        <v>35</v>
-      </c>
-      <c r="D803" t="s">
+      <c r="B802" t="s">
+        <v>339</v>
+      </c>
+      <c r="C802" t="s">
+        <v>55</v>
+      </c>
+      <c r="D802" t="s">
         <v>1842</v>
       </c>
-      <c r="E803" t="s">
-        <v>1843</v>
-      </c>
-      <c r="F803" t="s">
-        <v>42</v>
-      </c>
-      <c r="G803">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59136b72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J803" t="s">
-        <v>1844</v>
-      </c>
-      <c r="K803" t="s">
-        <v>1845</v>
-      </c>
-      <c r="M803" t="s">
-        <v>42</v>
+      <c r="E802" t="s">
+        <v>340</v>
+      </c>
+      <c r="F802" t="s">
+        <v>202</v>
+      </c>
+      <c r="G802">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912a516-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J802" t="s">
+        <v>341</v>
+      </c>
+      <c r="K802" t="s">
+        <v>91</v>
+      </c>
+      <c r="M802" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="804" spans="1:13">
       <c r="A804" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B804" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C804" t="s">
+        <v>35</v>
+      </c>
+      <c r="D804" t="s">
+        <v>1845</v>
+      </c>
+      <c r="E804" t="s">
         <v>1846</v>
-      </c>
-      <c r="C804" t="s">
-        <v>55</v>
-      </c>
-      <c r="D804" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E804" t="s">
-        <v>1848</v>
       </c>
       <c r="F804" t="s">
         <v>42</v>
       </c>
       <c r="G804">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2ca96cd5a4e83feb0d493bf9aa1a5b59.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59136b72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J804" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="K804" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="M804" t="s">
         <v>42</v>
@@ -31481,32 +31490,32 @@
     </row>
     <row r="805" spans="1:13">
       <c r="A805" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B805" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="C805" t="s">
         <v>55</v>
       </c>
       <c r="D805" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
       <c r="E805" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
       <c r="F805" t="s">
         <v>42</v>
       </c>
       <c r="G805">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/351c26a0f5a0cefa8f1183f2f12e1aa3.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2ca96cd5a4e83feb0d493bf9aa1a5b59.html","web")</f>
         <v>0</v>
       </c>
       <c r="J805" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="K805" t="s">
-        <v>1850</v>
+        <v>1853</v>
       </c>
       <c r="M805" t="s">
         <v>42</v>
@@ -31514,65 +31523,65 @@
     </row>
     <row r="806" spans="1:13">
       <c r="A806" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B806" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C806" t="s">
+        <v>55</v>
+      </c>
+      <c r="D806" t="s">
         <v>1855</v>
-      </c>
-      <c r="C806" t="s">
-        <v>35</v>
-      </c>
-      <c r="D806" t="s">
-        <v>172</v>
       </c>
       <c r="E806" t="s">
         <v>1856</v>
       </c>
       <c r="F806" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="G806">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15fea217c64dbec48b115765548b89ae.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/351c26a0f5a0cefa8f1183f2f12e1aa3.html","web")</f>
         <v>0</v>
       </c>
       <c r="J806" t="s">
         <v>1857</v>
       </c>
       <c r="K806" t="s">
-        <v>1858</v>
+        <v>1853</v>
       </c>
       <c r="M806" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
     </row>
     <row r="807" spans="1:13">
       <c r="A807" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B807" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="C807" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D807" t="s">
         <v>172</v>
       </c>
       <c r="E807" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="F807" t="s">
         <v>202</v>
       </c>
       <c r="G807">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/df06d844bd95ddd2f0f62f54941c4b88.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15fea217c64dbec48b115765548b89ae.html","web")</f>
         <v>0</v>
       </c>
       <c r="J807" t="s">
+        <v>1860</v>
+      </c>
+      <c r="K807" t="s">
         <v>1861</v>
-      </c>
-      <c r="K807" t="s">
-        <v>1862</v>
       </c>
       <c r="M807" t="s">
         <v>202</v>
@@ -31580,10 +31589,10 @@
     </row>
     <row r="808" spans="1:13">
       <c r="A808" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B808" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="C808" t="s">
         <v>55</v>
@@ -31592,20 +31601,20 @@
         <v>172</v>
       </c>
       <c r="E808" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="F808" t="s">
         <v>202</v>
       </c>
       <c r="G808">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/091b217c2450d012fb2e192dee04053f.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/df06d844bd95ddd2f0f62f54941c4b88.html","web")</f>
         <v>0</v>
       </c>
       <c r="J808" t="s">
+        <v>1864</v>
+      </c>
+      <c r="K808" t="s">
         <v>1865</v>
-      </c>
-      <c r="K808" t="s">
-        <v>1862</v>
       </c>
       <c r="M808" t="s">
         <v>202</v>
@@ -31613,7 +31622,7 @@
     </row>
     <row r="809" spans="1:13">
       <c r="A809" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B809" t="s">
         <v>1866</v>
@@ -31631,14 +31640,14 @@
         <v>202</v>
       </c>
       <c r="G809">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fb5bd0286cdca991d0f67c498513f602.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/091b217c2450d012fb2e192dee04053f.html","web")</f>
         <v>0</v>
       </c>
       <c r="J809" t="s">
         <v>1868</v>
       </c>
       <c r="K809" t="s">
-        <v>1508</v>
+        <v>1865</v>
       </c>
       <c r="M809" t="s">
         <v>202</v>
@@ -31646,7 +31655,7 @@
     </row>
     <row r="810" spans="1:13">
       <c r="A810" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B810" t="s">
         <v>1869</v>
@@ -31655,53 +31664,53 @@
         <v>55</v>
       </c>
       <c r="D810" t="s">
+        <v>172</v>
+      </c>
+      <c r="E810" t="s">
         <v>1870</v>
       </c>
-      <c r="E810" t="s">
+      <c r="F810" t="s">
+        <v>202</v>
+      </c>
+      <c r="G810">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fb5bd0286cdca991d0f67c498513f602.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J810" t="s">
         <v>1871</v>
-      </c>
-      <c r="F810" t="s">
-        <v>42</v>
-      </c>
-      <c r="G810">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/374e24b1cf7c24eb75126ea6e39ac478.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="J810" t="s">
-        <v>1872</v>
       </c>
       <c r="K810" t="s">
         <v>1508</v>
       </c>
       <c r="M810" t="s">
-        <v>42</v>
+        <v>202</v>
       </c>
     </row>
     <row r="811" spans="1:13">
       <c r="A811" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B811" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="C811" t="s">
         <v>55</v>
       </c>
       <c r="D811" t="s">
+        <v>1873</v>
+      </c>
+      <c r="E811" t="s">
         <v>1874</v>
-      </c>
-      <c r="E811" t="s">
-        <v>1875</v>
       </c>
       <c r="F811" t="s">
         <v>42</v>
       </c>
       <c r="G811">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1e93ae651487e683206b923c11fd6db1.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/374e24b1cf7c24eb75126ea6e39ac478.html","web")</f>
         <v>0</v>
       </c>
       <c r="J811" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="K811" t="s">
         <v>1508</v>
@@ -31712,29 +31721,29 @@
     </row>
     <row r="812" spans="1:13">
       <c r="A812" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B812" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="C812" t="s">
         <v>55</v>
       </c>
       <c r="D812" t="s">
+        <v>1877</v>
+      </c>
+      <c r="E812" t="s">
         <v>1878</v>
-      </c>
-      <c r="E812" t="s">
-        <v>1879</v>
       </c>
       <c r="F812" t="s">
         <v>42</v>
       </c>
       <c r="G812">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9289080901a39eba6ade178d596795a.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1e93ae651487e683206b923c11fd6db1.html","web")</f>
         <v>0</v>
       </c>
       <c r="J812" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="K812" t="s">
         <v>1508</v>
@@ -31745,34 +31754,67 @@
     </row>
     <row r="813" spans="1:13">
       <c r="A813" t="s">
-        <v>1840</v>
+        <v>1843</v>
       </c>
       <c r="B813" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="C813" t="s">
         <v>55</v>
       </c>
       <c r="D813" t="s">
+        <v>1881</v>
+      </c>
+      <c r="E813" t="s">
         <v>1882</v>
-      </c>
-      <c r="E813" t="s">
-        <v>1883</v>
       </c>
       <c r="F813" t="s">
         <v>42</v>
       </c>
       <c r="G813">
-        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b28e47214f0b71847c966828df0837ff.html","web")</f>
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9289080901a39eba6ade178d596795a.html","web")</f>
         <v>0</v>
       </c>
       <c r="J813" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="K813" t="s">
         <v>1508</v>
       </c>
       <c r="M813" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="814" spans="1:13">
+      <c r="A814" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B814" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C814" t="s">
+        <v>55</v>
+      </c>
+      <c r="D814" t="s">
+        <v>1885</v>
+      </c>
+      <c r="E814" t="s">
+        <v>1886</v>
+      </c>
+      <c r="F814" t="s">
+        <v>42</v>
+      </c>
+      <c r="G814">
+        <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b28e47214f0b71847c966828df0837ff.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="J814" t="s">
+        <v>1887</v>
+      </c>
+      <c r="K814" t="s">
+        <v>1508</v>
+      </c>
+      <c r="M814" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>